<commit_message>
requested publication of single record on test database
</commit_message>
<xml_diff>
--- a/scheduled_scripts/cuahsi/cuahsi_metadata.xlsx
+++ b/scheduled_scripts/cuahsi/cuahsi_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="891" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="891" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="587">
   <si>
     <t>How to Use this Guide</t>
   </si>
@@ -729,6 +729,9 @@
     <t>Luminous Flux</t>
   </si>
   <si>
+    <t>LUX</t>
+  </si>
+  <si>
     <t>Light2_lux</t>
   </si>
   <si>
@@ -1461,6 +1464,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ﾖ </t>
     </r>
@@ -2132,7 +2136,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2204,14 +2208,9 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2306,7 +2305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2403,10 +2402,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2419,7 +2414,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2435,11 +2430,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2794,53 +2789,53 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>529</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>530</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>531</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>532</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>533</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="H1" s="25" t="s">
+      <c r="F1" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>534</v>
-      </c>
-      <c r="J1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>535</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="J1" s="25" t="s">
         <v>536</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>537</v>
       </c>
-      <c r="M1" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="O1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>538</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="M1" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="O1" s="25" t="s">
         <v>539</v>
       </c>
-      <c r="Q1" s="25" t="s">
-        <v>512</v>
+      <c r="P1" s="25" t="s">
+        <v>540</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,46 +2849,46 @@
         <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>63</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>63</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>60</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,13 +2920,13 @@
         <v>10</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>66</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>66</v>
@@ -2940,7 +2935,7 @@
         <v>66</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>10</v>
@@ -2954,52 +2949,52 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>68</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3010,16 +3005,16 @@
         <v>81</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>81</v>
@@ -3028,31 +3023,31 @@
         <v>81</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="N5" s="0" t="s">
         <v>81</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q5" s="34" t="s">
-        <v>558</v>
+        <v>184</v>
+      </c>
+      <c r="Q5" s="33" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -3088,16 +3083,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>559</v>
-      </c>
-      <c r="B1" s="35" t="s">
+        <v>560</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>529</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>560</v>
+      <c r="C1" s="34" t="s">
+        <v>530</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,27 +3100,27 @@
         <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>494</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>507</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>507</v>
+      <c r="B3" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>508</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3136,10 +3131,10 @@
         <v>68</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3147,13 +3142,13 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3190,11 +3185,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>539</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>563</v>
+      <c r="B1" s="24" t="s">
+        <v>540</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,32 +3197,32 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,10 +3230,10 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3275,11 +3270,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>566</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>567</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3287,20 +3282,20 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>569</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="29" t="s">
+        <v>570</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3309,10 +3304,10 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,10 +3315,10 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3359,11 +3354,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>566</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>563</v>
+      <c r="B1" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3371,10 +3366,10 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3382,21 +3377,21 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3404,10 +3399,10 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3444,11 +3439,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>574</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>575</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,32 +3451,32 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,10 +3484,10 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3529,11 +3524,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>537</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>578</v>
+      <c r="B1" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3544,7 +3539,7 @@
         <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,21 +3547,21 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3574,34 +3569,34 @@
         <v>80</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="37" t="n">
+      <c r="B6" s="36" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -4240,8 +4235,8 @@
   </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4930,7 +4925,7 @@
         <v>82</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>89</v>
@@ -4959,7 +4954,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>131</v>
@@ -4968,7 +4963,7 @@
         <v>82</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>89</v>
@@ -4997,16 +4992,16 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>89</v>
@@ -5035,7 +5030,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>120</v>
@@ -5073,16 +5068,16 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>89</v>
@@ -5111,7 +5106,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>95</v>
@@ -5149,7 +5144,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>95</v>
@@ -5187,16 +5182,16 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>89</v>
@@ -5225,16 +5220,16 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>89</v>
@@ -5263,16 +5258,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>89</v>
@@ -5301,16 +5296,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>89</v>
@@ -5339,7 +5334,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>117</v>
@@ -5377,7 +5372,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>103</v>
@@ -5386,7 +5381,7 @@
         <v>82</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>89</v>
@@ -5415,7 +5410,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>116</v>
@@ -5424,7 +5419,7 @@
         <v>82</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>89</v>
@@ -5453,7 +5448,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>116</v>
@@ -5462,7 +5457,7 @@
         <v>82</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>89</v>
@@ -5491,7 +5486,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>112</v>
@@ -5500,7 +5495,7 @@
         <v>113</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>89</v>
@@ -5529,16 +5524,16 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>89</v>
@@ -5567,7 +5562,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>131</v>
@@ -5576,7 +5571,7 @@
         <v>82</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>89</v>
@@ -5605,7 +5600,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>131</v>
@@ -5614,7 +5609,7 @@
         <v>82</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>89</v>
@@ -5643,7 +5638,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>131</v>
@@ -5652,7 +5647,7 @@
         <v>82</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>89</v>
@@ -5681,16 +5676,16 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F38" s="21" t="s">
         <v>89</v>
@@ -5719,16 +5714,16 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>89</v>
@@ -5757,16 +5752,16 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="21" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>89</v>
@@ -5795,16 +5790,16 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>89</v>
@@ -5832,17 +5827,17 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="24" t="s">
-        <v>171</v>
+      <c r="B42" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>89</v>
@@ -5871,16 +5866,16 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>82</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>89</v>
@@ -5942,14 +5937,14 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>177</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5960,10 +5955,10 @@
         <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5985,13 +5980,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6005,106 +6000,106 @@
         <v>81</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -6136,8 +6131,8 @@
   </sheetPr>
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
@@ -6164,50 +6159,50 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="J1" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="M1" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="N1" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="O1" s="25" t="s">
         <v>224</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6227,7 +6222,7 @@
         <v>63</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>63</v>
@@ -6242,7 +6237,7 @@
         <v>63</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>63</v>
@@ -6254,10 +6249,10 @@
         <v>61</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6265,16 +6260,16 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>66</v>
@@ -6283,7 +6278,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>10</v>
@@ -6292,16 +6287,16 @@
         <v>10</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>10</v>
@@ -6312,49 +6307,49 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6368,48 +6363,48 @@
         <v>81</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>83</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>36.1359</v>
@@ -6418,24 +6413,24 @@
         <v>-79.1588</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>36.0715</v>
@@ -6444,22 +6439,22 @@
         <v>-79.0968</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>36.004</v>
@@ -6468,22 +6463,22 @@
         <v>-78.9715</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>35.9925</v>
@@ -6492,22 +6487,22 @@
         <v>-79.046</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>35.9795</v>
@@ -6516,22 +6511,22 @@
         <v>-79.0018</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>36.0325</v>
@@ -6540,22 +6535,22 @@
         <v>-79.0824</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>33.7532</v>
@@ -6564,27 +6559,24 @@
         <v>-111.506</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>34.8616</v>
@@ -6593,27 +6585,24 @@
         <v>-111.762</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>34.6793</v>
@@ -6622,27 +6611,24 @@
         <v>-111.695</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>33.5586</v>
@@ -6651,27 +6637,24 @@
         <v>-111.669</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>34.2561</v>
@@ -6680,27 +6663,24 @@
         <v>-112.066</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>29.8493</v>
@@ -6709,27 +6689,24 @@
         <v>-82.7148</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>29.8465</v>
@@ -6738,27 +6715,24 @@
         <v>-82.2197</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>29.998</v>
@@ -6767,27 +6741,24 @@
         <v>-82.2742</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>29.9219</v>
@@ -6796,27 +6767,24 @@
         <v>-82.4262</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>290</v>
+        <v>251</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>29.9526</v>
@@ -6825,27 +6793,24 @@
         <v>-82.7863</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>29.9118</v>
@@ -6854,27 +6819,24 @@
         <v>-82.8606</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>18.3213</v>
@@ -6883,24 +6845,21 @@
         <v>-65.8171</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>18.2754</v>
@@ -6909,27 +6868,24 @@
         <v>-65.7855</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L24" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="M24" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="M24" s="0" t="s">
-        <v>301</v>
-      </c>
       <c r="O24" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>41.7555</v>
@@ -6938,27 +6894,24 @@
         <v>-72.887</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>305</v>
+        <v>251</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>41.9083</v>
@@ -6967,27 +6920,24 @@
         <v>-72.7594</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L26" s="0" t="s">
-        <v>309</v>
+        <v>251</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>44.3656</v>
@@ -6996,27 +6946,24 @@
         <v>-72.0393</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>312</v>
+        <v>251</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>41.7862</v>
@@ -7025,27 +6972,24 @@
         <v>-72.9648</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L28" s="0" t="s">
-        <v>316</v>
+        <v>251</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>41.9679</v>
@@ -7054,27 +6998,24 @@
         <v>-73.0334</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>319</v>
+        <v>251</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>42.0375</v>
@@ -7083,27 +7024,24 @@
         <v>-72.9393</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>322</v>
+        <v>251</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C31" s="28" t="s">
         <v>326</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>327</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>44.4353</v>
@@ -7112,27 +7050,24 @@
         <v>-72.0389</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L31" s="0" t="s">
-        <v>325</v>
+        <v>251</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="P31" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>44.4761</v>
@@ -7141,27 +7076,24 @@
         <v>-72.125</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L32" s="0" t="s">
-        <v>328</v>
+        <v>251</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="P32" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>44.5117</v>
@@ -7170,27 +7102,24 @@
         <v>-71.8378</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>331</v>
+        <v>251</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="P33" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>43.1097</v>
@@ -7199,27 +7128,24 @@
         <v>-89.6408</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>334</v>
+        <v>251</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="P34" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>43.125</v>
@@ -7228,27 +7154,24 @@
         <v>-89.635</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>338</v>
+        <v>251</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="P35" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>41.8038</v>
@@ -7257,27 +7180,24 @@
         <v>-71.6499</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L36" s="0" t="s">
-        <v>341</v>
+        <v>251</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="P36" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>39.4797</v>
@@ -7286,24 +7206,21 @@
         <v>-76.6786</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L37" s="0" t="s">
-        <v>345</v>
+        <v>251</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P37" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>39.3112</v>
@@ -7312,24 +7229,21 @@
         <v>-76.7166</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L38" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="M38" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="M38" s="0" t="s">
-        <v>347</v>
-      </c>
       <c r="P38" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>39.4803</v>
@@ -7338,24 +7252,21 @@
         <v>-76.6875</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L39" s="0" t="s">
-        <v>350</v>
+        <v>251</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P39" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>39.2715</v>
@@ -7364,24 +7275,21 @@
         <v>-76.6486</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L40" s="0" t="s">
-        <v>352</v>
+        <v>251</v>
       </c>
       <c r="M40" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P40" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>39.4429</v>
@@ -7390,24 +7298,21 @@
         <v>-76.7834</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L41" s="0" t="s">
-        <v>354</v>
+        <v>251</v>
       </c>
       <c r="M41" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P41" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>39.3459</v>
@@ -7416,24 +7321,21 @@
         <v>-76.7332</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L42" s="0" t="s">
-        <v>356</v>
+        <v>251</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P42" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>34.4992</v>
@@ -7442,27 +7344,24 @@
         <v>-111.817</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L43" s="0" t="s">
-        <v>358</v>
+        <v>251</v>
       </c>
       <c r="M43" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O43" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="P43" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>18.2765</v>
@@ -7471,24 +7370,21 @@
         <v>-65.7859</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L44" s="0" t="s">
-        <v>361</v>
+        <v>251</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P44" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>18.324</v>
@@ -7497,24 +7393,21 @@
         <v>-65.8151</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L45" s="0" t="s">
-        <v>363</v>
+        <v>251</v>
       </c>
       <c r="M45" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P45" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>43.0933</v>
@@ -7523,24 +7416,21 @@
         <v>-70.989</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L46" s="0" t="s">
-        <v>365</v>
+        <v>251</v>
       </c>
       <c r="M46" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P46" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>44.0617</v>
@@ -7549,24 +7439,21 @@
         <v>-71.2946</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L47" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="M47" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="M47" s="0" t="s">
-        <v>367</v>
-      </c>
       <c r="P47" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>43.1347</v>
@@ -7575,24 +7462,21 @@
         <v>-71.1839</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L48" s="0" t="s">
-        <v>370</v>
+        <v>251</v>
       </c>
       <c r="M48" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P48" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>42.9481</v>
@@ -7601,27 +7485,24 @@
         <v>-71.4633</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L49" s="0" t="s">
-        <v>372</v>
+        <v>251</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="O49" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="P49" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>43.9549</v>
@@ -7630,24 +7511,21 @@
         <v>-71.7225</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L50" s="0" t="s">
-        <v>375</v>
+        <v>251</v>
       </c>
       <c r="M50" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P50" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>42.9648</v>
@@ -7656,24 +7534,21 @@
         <v>-71.478</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L51" s="0" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="M51" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P51" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>43.1704</v>
@@ -7682,24 +7557,21 @@
         <v>-71.2173</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L52" s="0" t="s">
-        <v>379</v>
+        <v>251</v>
       </c>
       <c r="M52" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P52" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>43.3178</v>
@@ -7708,24 +7580,21 @@
         <v>-71.1675</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L53" s="0" t="s">
-        <v>381</v>
+        <v>251</v>
       </c>
       <c r="M53" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P53" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>43.1222</v>
@@ -7734,24 +7603,21 @@
         <v>-71.0049</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L54" s="0" t="s">
-        <v>383</v>
+        <v>251</v>
       </c>
       <c r="M54" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P54" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>36.0573</v>
@@ -7760,27 +7626,24 @@
         <v>-78.9785</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L55" s="0" t="s">
-        <v>385</v>
+        <v>251</v>
       </c>
       <c r="M55" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="O55" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="P55" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>10.41</v>
@@ -7789,13 +7652,10 @@
         <v>-84.01</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="L56" s="0" t="s">
-        <v>388</v>
+        <v>251</v>
       </c>
       <c r="P56" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -7841,56 +7701,56 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>391</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="25" t="s">
         <v>394</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="K1" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="L1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="K1" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="N1" s="26" t="s">
         <v>402</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="O1" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="Q1" s="24" t="s">
         <v>405</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7904,10 +7764,10 @@
         <v>61</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>61</v>
@@ -7931,7 +7791,7 @@
         <v>61</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>61</v>
@@ -7940,13 +7800,13 @@
         <v>61</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>61</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7957,7 +7817,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>8</v>
@@ -7966,25 +7826,25 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>8</v>
@@ -7993,13 +7853,13 @@
         <v>66</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>10</v>
@@ -8010,55 +7870,55 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8075,7 +7935,7 @@
         <v>81</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>83</v>
@@ -8114,280 +7974,280 @@
         <v>83</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="C6" s="30" t="s">
         <v>426</v>
       </c>
+      <c r="C6" s="29" t="s">
+        <v>427</v>
+      </c>
       <c r="D6" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E6" s="21"/>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="L6" s="30" t="n">
+        <v>85287</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="L7" s="30" t="n">
+        <v>27708</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="R7" s="21"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="29" t="s">
+        <v>445</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="L8" s="30" t="n">
+        <v>32611</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="21"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>428</v>
       </c>
-      <c r="G6" s="30" t="s">
-        <v>429</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>430</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>431</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>432</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>433</v>
-      </c>
-      <c r="L6" s="31" t="n">
-        <v>85287</v>
-      </c>
-      <c r="M6" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="O6" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q6" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="30" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>460</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="29" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>436</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="30" t="s">
+      <c r="O9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="R9" s="21"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="G7" s="30" t="s">
-        <v>439</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="L7" s="31" t="n">
-        <v>27708</v>
-      </c>
-      <c r="M7" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="O7" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q7" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="R7" s="21"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="30" t="s">
-        <v>444</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="30" t="s">
-        <v>446</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>448</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>449</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>450</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>451</v>
-      </c>
-      <c r="L8" s="31" t="n">
-        <v>32611</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="O8" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="P8" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q8" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="R8" s="21"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="30" t="s">
-        <v>452</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>453</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="30" t="s">
-        <v>454</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>455</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>456</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>457</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>458</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>459</v>
-      </c>
-      <c r="M9" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="O9" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="P9" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q9" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="R9" s="21"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="30" t="s">
-        <v>460</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>437</v>
-      </c>
       <c r="E10" s="21"/>
-      <c r="F10" s="30" t="s">
-        <v>462</v>
-      </c>
-      <c r="G10" s="30" t="s">
+      <c r="F10" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="J10" s="29" t="s">
         <v>467</v>
       </c>
-      <c r="L10" s="31" t="n">
+      <c r="K10" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="L10" s="30" t="n">
         <v>53705</v>
       </c>
-      <c r="M10" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N10" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="O10" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="P10" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q10" s="30" t="s">
+      <c r="M10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="O10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q10" s="29" t="s">
         <v>83</v>
       </c>
       <c r="R10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="21" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>83</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>83</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>83</v>
@@ -8396,7 +8256,7 @@
         <v>83</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>83</v>
@@ -8410,31 +8270,31 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="21" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>83</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H12" s="32" t="s">
-        <v>477</v>
+      <c r="H12" s="31" t="s">
+        <v>478</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>83</v>
@@ -8443,7 +8303,7 @@
         <v>83</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O12" s="0" t="s">
         <v>83</v>
@@ -8457,31 +8317,31 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="21" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>83</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="33" t="s">
-        <v>483</v>
+      <c r="H13" s="32" t="s">
+        <v>484</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>83</v>
@@ -8490,7 +8350,7 @@
         <v>83</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O13" s="0" t="s">
         <v>83</v>
@@ -8504,10 +8364,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="21" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>83</v>
@@ -8537,7 +8397,7 @@
         <v>83</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O14" s="0" t="s">
         <v>83</v>
@@ -8551,10 +8411,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="21" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>83</v>
@@ -8584,7 +8444,7 @@
         <v>83</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O15" s="0" t="s">
         <v>83</v>
@@ -8638,14 +8498,14 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>490</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>491</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>492</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8659,7 +8519,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8667,13 +8527,13 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" s="21" customFormat="true" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8681,13 +8541,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8701,7 +8561,7 @@
         <v>81</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -8739,20 +8599,20 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>503</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="D1" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>504</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8769,10 +8629,10 @@
         <v>61</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8780,16 +8640,16 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
@@ -8800,19 +8660,19 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8832,7 +8692,7 @@
         <v>83</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -8869,14 +8729,14 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>512</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>513</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>514</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8890,7 +8750,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8898,10 +8758,10 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>8</v>
@@ -8912,13 +8772,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8926,68 +8786,68 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="30" t="n">
+      <c r="B6" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>519</v>
+      <c r="C6" s="29" t="s">
+        <v>520</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="30" t="n">
+      <c r="B7" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>521</v>
+      <c r="C7" s="29" t="s">
+        <v>522</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="30" t="n">
+      <c r="B8" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>523</v>
+      <c r="C8" s="29" t="s">
+        <v>524</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="30" t="n">
+      <c r="B9" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>525</v>
+      <c r="C9" s="29" t="s">
+        <v>526</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="30" t="n">
+      <c r="B10" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>527</v>
+      <c r="C10" s="29" t="s">
+        <v>528</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>